<commit_message>
CCRU - Template Example update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/CCRU_VisitPlan_Example.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/CCRU_VisitPlan_Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="planned_visits" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,9 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">1 – for planned Sales Reps visits
-0 – to exclude non-SalesReps visits from “planned”</t>
+0 – to exclude non-SalesReps visits from “planned”
+Row 1 – Headres
+Row 2-3 – Period limits</t>
         </r>
       </text>
     </comment>
@@ -81,9 +83,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,13 +108,27 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,16 +165,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,112 +202,116 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2672064777328"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6882591093117"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="n">
         <v>43485</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="n">
         <v>43496</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3800001017</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="1" t="n">
         <v>43439</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3800001017</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="1" t="n">
         <v>43495</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>3800001141</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="1" t="n">
         <v>43455</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>3800001141</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="1" t="n">
         <v>43490</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>3800001141</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="1" t="n">
         <v>43497</v>
       </c>
       <c r="D8" s="0" t="n">

</xml_diff>